<commit_message>
Final Changes for new FVA Job type(PRJ0019112)
</commit_message>
<xml_diff>
--- a/TestData/T1592_ValidationsToBeCompleted.xlsx
+++ b/TestData/T1592_ValidationsToBeCompleted.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgoyal0427\source\repos\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VKumar0427\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7DC96DB-B98A-455A-B673-28DE964914BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="8640" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddOpportunity" sheetId="1" r:id="rId1"/>
@@ -22,20 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="106">
   <si>
     <t>Client</t>
   </si>
@@ -157,9 +150,6 @@
     <t>10.0</t>
   </si>
   <si>
-    <t>9999.0</t>
-  </si>
-  <si>
     <t>Board of Directors</t>
   </si>
   <si>
@@ -350,12 +340,18 @@
   </si>
   <si>
     <t>Opportunity Detail - SIC Code., Opportunity Description - Opportunity Description., Estimated Financials - Est. Transaction Size/Market Cap., Estimated Fees - Retainer, input zero if there's no Retainer fee., Estimated Fees - Tail Expires., Estimated Fees - Progress/Monthly Fee., Estimated Fees - Contingent Fee., Referral Information - Referral Contact name is required., HL Internal Team - Team must include the following roles: Initiator, Seller, Principal, Manager, Associate(Optional), Analyst(Optional)., Legal Matters - Confidentiality Agreement, Conflicts Check - A Conflicts Check was completed more than 30 days ago. A new Conflicts Check must be completed., Administration - Estimated Closed Date., Administration - "Women Led" is required. Please update this field with the correct value, Administration - Fairness Opinion Component., Administration - Date Engaged - Date of Executed Retainer or similar document., Approved NBC form - Please complete and submit this form via the NBC button., Opportunity Contacts - Add at least one Primary Opportunity Contact., Opportunity Contacts - Add at least one Billing Contact.</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>9999</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -399,11 +395,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -706,210 +700,206 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AE6" sqref="AE6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" style="3"/>
-    <col min="3" max="3" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="3"/>
-    <col min="15" max="17" width="14.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="27" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="8.85546875" style="3"/>
-    <col min="26" max="26" width="11.28515625" style="3" customWidth="1"/>
-    <col min="27" max="16384" width="8.85546875" style="3"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" t="s">
+        <v>99</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="R2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="U2" t="s">
+        <v>31</v>
+      </c>
+      <c r="V2" t="s">
+        <v>100</v>
+      </c>
+      <c r="W2" t="s">
+        <v>34</v>
+      </c>
+      <c r="X2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z2" t="s">
         <v>44</v>
       </c>
-      <c r="AA1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB2" s="5" t="s">
-        <v>39</v>
+      <c r="AA2" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -919,7 +909,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -941,11 +931,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>100</v>
+      <c r="A2" t="s">
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -954,10 +944,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -975,73 +965,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="11" t="s">
+      <c r="C1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="H1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="162" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="E2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="11" t="s">
+      <c r="G2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="162" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="I2" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="7" t="s">
         <v>102</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1051,7 +1041,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AF33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1060,318 +1050,318 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="95.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="10"/>
-    <col min="8" max="8" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="8.85546875" style="10"/>
-    <col min="13" max="13" width="10.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="5"/>
-    <col min="15" max="16" width="8.85546875" style="10"/>
-    <col min="17" max="17" width="10.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="29.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="8.85546875" style="10"/>
-    <col min="21" max="21" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.85546875" style="10"/>
-    <col min="23" max="23" width="13.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="30" width="8.85546875" style="10"/>
-    <col min="31" max="31" width="10.5703125" style="10" customWidth="1"/>
-    <col min="32" max="32" width="102.28515625" style="10" customWidth="1"/>
-    <col min="33" max="16384" width="8.85546875" style="10"/>
+    <col min="1" max="1" width="95.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="8"/>
+    <col min="8" max="8" width="12.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="8.85546875" style="8"/>
+    <col min="13" max="13" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="3"/>
+    <col min="15" max="16" width="8.85546875" style="8"/>
+    <col min="17" max="17" width="10.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="8.85546875" style="8"/>
+    <col min="21" max="21" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" style="8"/>
+    <col min="23" max="23" width="13.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="30" width="8.85546875" style="8"/>
+    <col min="31" max="31" width="10.5703125" style="8" customWidth="1"/>
+    <col min="32" max="32" width="102.28515625" style="8" customWidth="1"/>
+    <col min="33" max="16384" width="8.85546875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="V1" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="W1" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="X1" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z1" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA1" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB1" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC1" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD1" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE1" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="AF1" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="O1" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="R1" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="S1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="T1" s="11" t="s">
+      <c r="D2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="U1" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="V1" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="W1" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="X1" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y1" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="Z1" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="AA1" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB1" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="AC1" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="AD1" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE1" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF1" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" ht="144" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="S2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="V2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF2" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="R2" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="S2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="T2" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="U2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="V2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="W2" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="X2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y2" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF2" s="9" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="5"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="5"/>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="5"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="5"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="A7" s="5"/>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="5"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="5"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="5"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="5"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="5"/>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="5"/>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+      <c r="A14" s="5"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="5"/>
     </row>
     <row r="16" spans="1:32" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="5"/>
     </row>
     <row r="17" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+      <c r="A17" s="5"/>
     </row>
     <row r="18" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="A18" s="5"/>
     </row>
     <row r="19" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="5"/>
     </row>
     <row r="20" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+      <c r="A20" s="5"/>
     </row>
     <row r="21" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="5"/>
     </row>
     <row r="22" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
+      <c r="A22" s="5"/>
     </row>
     <row r="23" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
+      <c r="A23" s="5"/>
     </row>
     <row r="24" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
+      <c r="A24" s="5"/>
     </row>
     <row r="25" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
+      <c r="A25" s="5"/>
     </row>
     <row r="26" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
+      <c r="A26" s="5"/>
     </row>
     <row r="27" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
+      <c r="A27" s="5"/>
     </row>
     <row r="28" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
+      <c r="A28" s="5"/>
     </row>
     <row r="29" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
+      <c r="A29" s="5"/>
     </row>
     <row r="30" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
+      <c r="A30" s="5"/>
     </row>
     <row r="31" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
+      <c r="A31" s="5"/>
     </row>
     <row r="32" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
+      <c r="A32" s="5"/>
     </row>
     <row r="33" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
+      <c r="A33" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Opp to Eng validation and expense req changes
</commit_message>
<xml_diff>
--- a/TestData/T1592_ValidationsToBeCompleted.xlsx
+++ b/TestData/T1592_ValidationsToBeCompleted.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VKumar0427\source\repos\SF_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vijay.kumar\source\repos\SalesForce_Project\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7DC96DB-B98A-455A-B673-28DE964914BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34F64EA-C812-441A-B278-506BE36DED06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddOpportunity" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="108">
   <si>
     <t>Client</t>
   </si>
@@ -336,16 +336,22 @@
     <t>Error:, Estimated Financials - Client/Subject: EBITDA(MM), please provide a EBITDA(MM) value on the Client or Subject Company record in Company Financials</t>
   </si>
   <si>
-    <t>Opportunity Detail - Client: Street Address., Opportunity Detail - Client: City Address., Opportunity Detail - Client: Postal Code., Opportunity Detail - Subject: Street Address., Opportunity Detail - Subject: City Address., Opportunity Detail - Subject: Postal Code Address., Estimated Financials - Client/Subject: EBITDA(MM), please provide a EBITDA(MM) value on the Client or Subject Company record in Company Financials</t>
-  </si>
-  <si>
     <t>Opportunity Detail - SIC Code., Opportunity Description - Opportunity Description., Estimated Financials - Est. Transaction Size/Market Cap., Estimated Fees - Retainer, input zero if there's no Retainer fee., Estimated Fees - Tail Expires., Estimated Fees - Progress/Monthly Fee., Estimated Fees - Contingent Fee., Referral Information - Referral Contact name is required., HL Internal Team - Team must include the following roles: Initiator, Seller, Principal, Manager, Associate(Optional), Analyst(Optional)., Legal Matters - Confidentiality Agreement, Conflicts Check - A Conflicts Check was completed more than 30 days ago. A new Conflicts Check must be completed., Administration - Estimated Closed Date., Administration - "Women Led" is required. Please update this field with the correct value, Administration - Fairness Opinion Component., Administration - Date Engaged - Date of Executed Retainer or similar document., Approved NBC form - Please complete and submit this form via the NBC button., Opportunity Contacts - Add at least one Primary Opportunity Contact., Opportunity Contacts - Add at least one Billing Contact.</t>
   </si>
   <si>
+    <t>10000</t>
+  </si>
+  <si>
     <t>10</t>
   </si>
   <si>
     <t>9999</t>
+  </si>
+  <si>
+    <t>Estimated Financials - Client/Subject: EBITDA(MM), please provide a EBITDA(MM) value on the Client or Subject Company record in Company Financials</t>
+  </si>
+  <si>
+    <t>Opportunity Detail - Client: Street Address., Opportunity Detail - Client: City Address., Opportunity Detail - Client: Postal Code., Opportunity Detail - Subject: Street Address., Opportunity Detail - Subject: City Address., Opportunity Detail - Subject: Postal Code Address.</t>
   </si>
 </sst>
 </file>
@@ -703,34 +709,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AE6" sqref="AE6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="14.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5546875" style="4" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="21" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="27" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.28515625" customWidth="1"/>
+    <col min="26" max="26" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -816,7 +822,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -866,7 +872,7 @@
         <v>104</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="R2" t="s">
         <v>28</v>
@@ -916,13 +922,13 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -930,7 +936,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -945,26 +951,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="86.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="86.6640625" customWidth="1"/>
     <col min="10" max="10" width="45" customWidth="1"/>
-    <col min="11" max="11" width="54.42578125" customWidth="1"/>
+    <col min="11" max="11" width="54.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>37</v>
       </c>
@@ -999,7 +1005,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="162" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="162" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>100</v>
       </c>
@@ -1025,13 +1031,16 @@
         <v>57</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>101</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1048,33 +1057,33 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="95.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="8"/>
-    <col min="8" max="8" width="12.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="8.85546875" style="8"/>
-    <col min="13" max="13" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="3"/>
-    <col min="15" max="16" width="8.85546875" style="8"/>
-    <col min="17" max="17" width="10.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="29.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="8.85546875" style="8"/>
-    <col min="21" max="21" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.85546875" style="8"/>
-    <col min="23" max="23" width="13.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="24" max="30" width="8.85546875" style="8"/>
-    <col min="31" max="31" width="10.5703125" style="8" customWidth="1"/>
-    <col min="32" max="32" width="102.28515625" style="8" customWidth="1"/>
-    <col min="33" max="16384" width="8.85546875" style="8"/>
+    <col min="1" max="1" width="95.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="8"/>
+    <col min="8" max="8" width="12.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="8.88671875" style="8"/>
+    <col min="13" max="13" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" style="3"/>
+    <col min="15" max="16" width="8.88671875" style="8"/>
+    <col min="17" max="17" width="10.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="8.88671875" style="8"/>
+    <col min="21" max="21" width="9.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.88671875" style="8"/>
+    <col min="23" max="23" width="13.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="30" width="8.88671875" style="8"/>
+    <col min="31" max="31" width="10.5546875" style="8" customWidth="1"/>
+    <col min="32" max="32" width="102.33203125" style="8" customWidth="1"/>
+    <col min="33" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>58</v>
       </c>
@@ -1172,7 +1181,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" ht="144" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>93</v>
       </c>
@@ -1270,97 +1279,97 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
     </row>
-    <row r="16" spans="1:32" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
     </row>
-    <row r="17" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
     </row>
-    <row r="18" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
     </row>
-    <row r="19" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
     </row>
-    <row r="20" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
     </row>
-    <row r="21" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
     </row>
-    <row r="22" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
     </row>
-    <row r="23" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
     </row>
-    <row r="24" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
     </row>
-    <row r="25" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
     </row>
-    <row r="26" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
     </row>
-    <row r="27" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
     </row>
-    <row r="28" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
     </row>
-    <row r="29" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
     </row>
-    <row r="30" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
     </row>
-    <row r="31" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
     </row>
-    <row r="32" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
     </row>
-    <row r="33" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
     </row>
   </sheetData>

</xml_diff>